<commit_message>
Added export to JSON and yEd. Added extra large canvas checkbox. Minor fixes.
</commit_message>
<xml_diff>
--- a/cogs/cogsExample.xlsx
+++ b/cogs/cogsExample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Арагорн</t>
   </si>
@@ -39,9 +39,6 @@
     <t>предмет</t>
   </si>
   <si>
-    <t>Кольцо</t>
-  </si>
-  <si>
     <t>несет</t>
   </si>
   <si>
@@ -51,13 +48,16 @@
     <t>ищет</t>
   </si>
   <si>
-    <t>+юркий -слабый</t>
-  </si>
-  <si>
-    <t>+удачливый -старый</t>
-  </si>
-  <si>
-    <t>+бессмертный</t>
+    <t>Удачливый, старый</t>
+  </si>
+  <si>
+    <t>Юркий, слабый</t>
+  </si>
+  <si>
+    <t>бессмертный</t>
+  </si>
+  <si>
+    <t>убегает от</t>
   </si>
 </sst>
 </file>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -410,6 +410,7 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
+      <c r="C1"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -418,8 +419,8 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -429,7 +430,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -440,6 +441,7 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
@@ -448,8 +450,8 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -457,10 +459,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -468,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -479,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -487,12 +489,23 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>